<commit_message>
Added space to selenium dsl commands
</commit_message>
<xml_diff>
--- a/SampleProject/src/main/resources/Testcases.xlsx
+++ b/SampleProject/src/main/resources/Testcases.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="599"/>
@@ -16,69 +16,55 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Add 5 and 2 Assign %{result}%
 %{result}% VerifyEqual 7
 Print %{result}%</t>
   </si>
   <si>
-    <t>LoadUrl http://127.0.0.1/wordpress/wp-admin
+    <t>TC_001</t>
+  </si>
+  <si>
+    <t>TC_002</t>
+  </si>
+  <si>
+    <t>TC_003</t>
+  </si>
+  <si>
+    <t>Load Url http://en.wikipedia.org/wiki/India
+Click element with linkText = View history
+Sleep 5
+Get Page Title Assign %{title}%
+%{title}% VerifyEqual India: Revision history - Wikipedia, the free encyclopedia
+Quit Browser</t>
+  </si>
+  <si>
+    <t>Load Url http://127.0.0.1/wordpress/wp-admin
+Maximize Browser Window
 Sleep 2
-GetPageTitle Assign %{title}%
+Get Page Title Assign %{title}%
 %{title}% VerifyEqual test › Log In
-Print %{title}%</t>
-  </si>
-  <si>
-    <t>LoadUrl http://127.0.0.1/wordpress/wp-admin
+Print %{title}%
+Quit Browser</t>
+  </si>
+  <si>
+    <t>Invoke Browser
+Load Url http://127.0.0.1/wordpress/wp-admin
 Type admin in element with id = user_login
 Type test in element with id = user_pass
 Click element with id = wp-submit
 Sleep 2
-GetPageTitle Assign %{title}%
+Get Page Title Assign %{title}%
 %{title}% VerifyEqual Dashboard ‹ test — WordPress
-QuitBrowser</t>
-  </si>
-  <si>
-    <t>Add 5 and 3 Assign %{result}%
-%{result}% VerifyEqual 8
-Print %{result}%</t>
-  </si>
-  <si>
-    <t>LoadUrl http://127.0.0.1/wordpress/wp-admin
-MaximizeBrowserWindow
-Sleep 2
-GetPageTitle Assign %{title}%
-%{title}% VerifyEqual test › Log In
-Print %{title}%</t>
-  </si>
-  <si>
-    <t>LoadUrl http://127.0.0.1/wordpress/wp-admin
-Type admin in element with id = user_login
-Type test in element with id = user_pass
-Click element with id = wp-submit
-Sleep 2
-GetPageTitle Assign %{title}%
-%{title}% VerifyEqual Dashboard ‹ test — WordPress</t>
-  </si>
-  <si>
-    <t>LoadUrl http://en.wikipedia.org/wiki/India
-MaximizeBrowserWindow
-Click element with linkText = View history
-Sleep 5
-GetPageTitle Assign %{title}%
-%{title}% VerifyEqual India: Revision history - Wikipedia, the free encyclopedia
-QuitBrowser</t>
-  </si>
-  <si>
-    <t>TC_001</t>
+Quit Browser</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -103,41 +89,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -151,6 +113,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -229,6 +196,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -263,6 +231,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -438,60 +407,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="83.140625" style="1" customWidth="1"/>
-    <col min="3" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="71" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45">
-      <c r="A1" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="105">
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="45">
-      <c r="A3" s="6"/>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45.75" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="78" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="3" t="s">
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="105">
-      <c r="A6" s="6"/>
-      <c r="B6" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -500,38 +457,50 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" customWidth="1"/>
-    <col min="2" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="71" style="1" customWidth="1"/>
+    <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="75">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="120">
-      <c r="A2" s="5" t="s">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2"/>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1"/>
-    <row r="7" spans="1:2" ht="16.5" thickTop="1" thickBot="1">
-      <c r="A7" s="4"/>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" thickTop="1"/>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -539,12 +508,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1025" width="8.5703125"/>
   </cols>

</xml_diff>

<commit_message>
DSL commandsfor all selenium utilities and execution on multiple browser
</commit_message>
<xml_diff>
--- a/SampleProject/src/main/resources/Testcases.xlsx
+++ b/SampleProject/src/main/resources/Testcases.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="599"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>Add 5 and 2 Assign %{result}%
 %{result}% VerifyEqual 7
@@ -59,12 +60,96 @@
 %{title}% VerifyEqual Dashboard ‹ test — WordPress
 Quit Browser</t>
   </si>
+  <si>
+    <t>Invoke Browser
+Load Url http://127.0.0.1/wordpress/wp-admin
+Maximize Browser Window
+Sleep 2
+Get Page Title Assign %{title}%
+%{title}% VerifyEqual test › Log In
+Print %{title}%
+Quit Browser</t>
+  </si>
+  <si>
+    <t>Invoke Browser
+Load Url http://127.0.0.1/wordpress/wp-admin
+Type admin in element with id = user_login
+Type test in element with id = user_pass
+Click element with id = wp-submit
+Click element with xpath = //li[@id='menu-posts']/a/div[3]
+sleep 5
+Quit Browser</t>
+  </si>
+  <si>
+    <t>Invoke Browser
+Load Url http://127.0.0.1/wordpress/wp-admin
+Type admin in UserNameField with id = user_login
+Type test in PasswordField with id = user_pass
+Click LogInBtn with id = wp-submit
+Click PostsLink with xpath = //li[@id='menu-posts']/a/div[3]
+Select Edit from ActionsListBox with xpath = //form[@id='posts-filter']/div[1]/div[1]/select
+Quit Browser</t>
+  </si>
+  <si>
+    <t>Invoke Browser
+Load Url http://127.0.0.1/wordpress/wp-admin
+Type admin in UserNameField with id = user_login
+Type test in PasswordField with id = user_pass
+Get Tag Name of LogInBtn with id = wp-submit Assign %{LogInBtnTagName}%
+%{LogInBtnTagName}% VerifyEqual input
+Get Value of Attribute: value of LogInBtn with id = wp-submit  Assign %{LogInBtnValue}%
+%{LogInBtnValue}% VerifyEqual Log In
+Is LogInBtn with id = wp-submit Displayed Assign %{LogInBtnDisplayed}%
+%{LogInBtnDisplayed}% VerifyEqual true
+Is LogInBtn with id = wp-submit Enabled Assign %{LogInBtnEnabled}%
+%{LogInBtnEnabled}% VerifyEqual true
+Get Text of UserNameLabel with xpath = //form[@id='loginform']/p[1]/label Assign %{UserNameLabelText}%
+%{UserNameLabelText}% VerifyEqual  Username
+Is RememberMeChkBox with id = rememberme Selected Assign %{RememberMeSelected}%
+%{RememberMeSelected}% VerifyEqual false
+Click RememberMeChkBox with id = rememberme
+Is RememberMeChkBox with id = rememberme Selected Assign %{RememberMeSelected}%
+%{RememberMeSelected}% VerifyEqual true
+Click LogInBtn with id = wp-submit
+Get Page Title Assign %{title}%
+%{title}% VerifyEqual Dashboard ‹ test — WordPress
+Quit Browser</t>
+  </si>
+  <si>
+    <t>Invoke browser
+Load url http://127.0.0.1/wordpress/wp-admin
+Type admin in UserNameField with id = user_login
+Clear UserNameField with id = user_login
+Type admin in UserNameField with id = user_login
+Type test in PasswordField with id = user_pass
+Get tagname of LogInBtn with id = wp-submit Assign {LogInBtnTagName}
+{LogInBtnTagName} VerifyEqual input
+Get value of attribute: value of LogInBtn with id = wp-submit  Assign {LogInBtnValue}
+{LogInBtnValue} VerifyEqual Log In
+Is LogInBtn with id = wp-submit displayed Assign {LogInBtnDisplayed}
+{LogInBtnDisplayed} VerifyEqual true
+Is LogInBtn with id = wp-submit enabled Assign {LogInBtnEnabled}
+{LogInBtnEnabled} VerifyEqual true
+Get text of UserNameLabel with xpath = //form[@id='loginform']/p[1]/label Assign {UserNameLabelText}
+{UserNameLabelText} VerifyEqual  Username
+Is RememberMeChkBox with id = rememberme selected Assign {RememberMeSelected}
+{RememberMeSelected} VerifyEqual false
+Click RememberMeChkBox with id = rememberme
+Is RememberMeChkBox with id = rememberme selected Assign {RememberMeSelected}
+{RememberMeSelected} VerifyEqual true
+Click LogInBtn with id = wp-submit
+Get page title Assign {title}
+{title} VerifyEqual Dashboard ‹ test — WordPress
+Get current page url Assign {pageUrl}
+{pageUrl} VerifyEqual http://127.0.0.1/wordpress/wp-admin/
+Quit browser</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -196,7 +281,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -231,7 +315,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -407,47 +490,55 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="71" style="1" customWidth="1"/>
+    <col min="2" max="2" width="94.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="409.5" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="123.75" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="45">
+      <c r="A3" s="3"/>
+      <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="120">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="135">
+      <c r="A5" s="3"/>
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="120">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -457,21 +548,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
     <col min="2" max="2" width="71" style="1" customWidth="1"/>
     <col min="3" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="45">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -479,7 +570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="105">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -487,7 +578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="135">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -495,10 +586,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="105">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="405">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -508,12 +604,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1025" width="8.5703125"/>
   </cols>

</xml_diff>

<commit_message>
Implemented comments, enabling testcases, reading global config file
</commit_message>
<xml_diff>
--- a/SampleProject/src/main/resources/Testcases.xlsx
+++ b/SampleProject/src/main/resources/Testcases.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Add 5 and 2 Assign %{result}%
 %{result}% VerifyEqual 7
@@ -58,36 +57,6 @@
 Sleep 2
 Get Page Title Assign %{title}%
 %{title}% VerifyEqual Dashboard ‹ test — WordPress
-Quit Browser</t>
-  </si>
-  <si>
-    <t>Invoke Browser
-Load Url http://127.0.0.1/wordpress/wp-admin
-Maximize Browser Window
-Sleep 2
-Get Page Title Assign %{title}%
-%{title}% VerifyEqual test › Log In
-Print %{title}%
-Quit Browser</t>
-  </si>
-  <si>
-    <t>Invoke Browser
-Load Url http://127.0.0.1/wordpress/wp-admin
-Type admin in element with id = user_login
-Type test in element with id = user_pass
-Click element with id = wp-submit
-Click element with xpath = //li[@id='menu-posts']/a/div[3]
-sleep 5
-Quit Browser</t>
-  </si>
-  <si>
-    <t>Invoke Browser
-Load Url http://127.0.0.1/wordpress/wp-admin
-Type admin in UserNameField with id = user_login
-Type test in PasswordField with id = user_pass
-Click LogInBtn with id = wp-submit
-Click PostsLink with xpath = //li[@id='menu-posts']/a/div[3]
-Select Edit from ActionsListBox with xpath = //form[@id='posts-filter']/div[1]/div[1]/select
 Quit Browser</t>
   </si>
   <si>
@@ -116,8 +85,14 @@
 Quit Browser</t>
   </si>
   <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
     <t>Invoke browser
-Load url http://127.0.0.1/wordpress/wp-admin
+Load testUrl
 Type admin in UserNameField with id = user_login
 Clear UserNameField with id = user_login
 Type admin in UserNameField with id = user_login
@@ -143,6 +118,39 @@
 Get current page url Assign {pageUrl}
 {pageUrl} VerifyEqual http://127.0.0.1/wordpress/wp-admin/
 Quit browser</t>
+  </si>
+  <si>
+    <t>Invoke browser
+Load testUrl
+Type admin in UserNameField with id = user_login
+Type test in PasswordField with id = user_pass
+Click LogInBtn with id = wp-submit
+Type test post title in PostTitleField with id = title
+Type test post content in PostContentField with id = content
+Click PublishBtn with id = publish
+Sleep 2
+Is ViewPostLink with linkText = View post displayed Assign {ViewPostLinkDisplayed}
+{ViewPostLinkDisplayed} VerifyEqual true
+Is EditPostLink with linkText = Edit post displayed Assign {EditPostLinkDisplayed}
+{EditPostLinkDisplayed} VerifyEqual true
+Quit browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invoke browser
+Load testUrl
+Type admin in UserNameField with id = user_login
+Type test in PasswordField with id = user_pass
+Click LogInBtn with id = wp-submit
+Click PostsLink with xpath = //li[@id='menu-posts']/a/div[3]
+Get page title Assign {title}
+{title} VerifyEqual Posts ‹ test — WordPress
+Select Edit from ActionsListBox with xpath = //form[@id='posts-filter']/div[1]/div[1]/select
+Click AddedPostLink with xpath = //tr[contains(@id,'post')]/td[1]/strong/a
+Get page title Assign {title}
+{title} VerifyEqual Edit Post ‹ test — WordPress
+Click MoveToTrashLink with xpath = //div[@id='delete-action']/a
+Quit browser
+</t>
   </si>
 </sst>
 </file>
@@ -178,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -191,6 +199,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,54 +502,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="94.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="94.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="409.5" customHeight="1">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" ht="409.5" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="210">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="123.75" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="2" t="s">
+    <row r="3" spans="1:3" ht="225">
+      <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="45">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="120">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="135">
-      <c r="A5" s="3"/>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="120">
-      <c r="A6" s="3"/>
-      <c r="B6" s="2" t="s">
-        <v>8</v>
+      <c r="B3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +601,7 @@
     </row>
     <row r="5" spans="1:2" ht="405">
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Boolean Operation, If-Else control loop
</commit_message>
<xml_diff>
--- a/SampleProject/src/main/resources/Testcases.xlsx
+++ b/SampleProject/src/main/resources/Testcases.xlsx
@@ -157,17 +157,22 @@
   </si>
   <si>
     <t>Invoke browser
-Load testUrl
+Load {testUrl}
 Type admin in UserNameField with id = user_login
 Type test in PasswordField with id = user_pass
 Click LogInBtn with id = wp-submit
 Is SettingsSection with id = adv-settings displayed Assign {SettingsSectionDisplayed}
-{SettingsSectionDisplayed} VerifyEqual false
-Click ScreenOptionsBtn with id = show-settings-link
+If (not({SettingsSectionDisplayed}))
+  {SettingsSectionDisplayed} VerifyEqual false
+  Click ScreenOptionsBtn with id = show-settings-link
+End If
 Is SettingsSection with id = adv-settings displayed Assign {SettingsSectionDisplayed}
-If ({SettingsSectionDisplayed})
-{SettingsSectionDisplayed} VerifyEqual true
+If (not({SettingsSectionDisplayed}))
+  {SettingsSectionDisplayed} VerifyEqual true
 End If
+Else
+   Print {SettingsSectionDisplayed}
+End Else
 Quit browser</t>
   </si>
 </sst>
@@ -522,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -566,7 +571,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="195">
+    <row r="4" spans="1:3" ht="270">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
If and While Loop
</commit_message>
<xml_diff>
--- a/SampleProject/src/main/resources/Testcases.xlsx
+++ b/SampleProject/src/main/resources/Testcases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Add 5 and 2 Assign %{result}%
 %{result}% VerifyEqual 7
@@ -91,8 +91,11 @@
     <t>Disabled</t>
   </si>
   <si>
+    <t>TC_004</t>
+  </si>
+  <si>
     <t>Invoke browser
-Load testUrl
+Load {testUrl}
 Type admin in UserNameField with id = user_login
 Clear UserNameField with id = user_login
 Type admin in UserNameField with id = user_login
@@ -121,7 +124,7 @@
   </si>
   <si>
     <t>Invoke browser
-Load testUrl
+Load {testUrl}
 Type admin in UserNameField with id = user_login
 Type test in PasswordField with id = user_pass
 Click LogInBtn with id = wp-submit
@@ -137,7 +140,7 @@
   </si>
   <si>
     <t xml:space="preserve">Invoke browser
-Load testUrl
+Load {testUrl}
 Type admin in UserNameField with id = user_login
 Type test in PasswordField with id = user_pass
 Click LogInBtn with id = wp-submit
@@ -153,7 +156,7 @@
 </t>
   </si>
   <si>
-    <t>TC_004</t>
+    <t>TC_005</t>
   </si>
   <si>
     <t>Invoke browser
@@ -162,17 +165,36 @@
 Type test in PasswordField with id = user_pass
 Click LogInBtn with id = wp-submit
 Is SettingsSection with id = adv-settings displayed Assign {SettingsSectionDisplayed}
+Print {SettingsSectionDisplayed}
 If (not({SettingsSectionDisplayed}))
   {SettingsSectionDisplayed} VerifyEqual false
   Click ScreenOptionsBtn with id = show-settings-link
+  Sleep 2
 End If
 Is SettingsSection with id = adv-settings displayed Assign {SettingsSectionDisplayed}
-If (not({SettingsSectionDisplayed}))
-  {SettingsSectionDisplayed} VerifyEqual true
+If ({SettingsSectionDisplayed})
+  {SettingsSectionDisplayed} VerifyEqual true  
 End If
 Else
    Print {SettingsSectionDisplayed}
 End Else
+Quit browser</t>
+  </si>
+  <si>
+    <t>Invoke browser
+Load {testUrl}
+Type admin in UserNameField with id = user_login
+Type test in PasswordField with id = user_pass
+Click LogInBtn with id = wp-submit
+Click ScreenOptionsBtn with id = show-settings-link
+Is SettingsSection with id = adv-settings displayed Assign {SettingsSectionDisplayed}
+#Print {SettingsSectionDisplayed}
+While (({SettingsSectionDisplayed}))
+  {SettingsSectionDisplayed} VerifyEqual true  
+  Click ScreenOptionsBtn with id = show-settings-link
+  Is SettingsSection with id = adv-settings displayed Assign {SettingsSectionDisplayed}
+End While
+{SettingsSectionDisplayed} VerifyEqual false 
 Quit browser</t>
   </si>
 </sst>
@@ -525,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -546,7 +568,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="210">
@@ -557,7 +579,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="215.25" customHeight="1">
@@ -568,18 +590,29 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="270">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="300">
       <c r="A4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="225">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>14</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -593,7 +626,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added additional commands and modified testcase excel
</commit_message>
<xml_diff>
--- a/SampleProject/src/main/resources/Testcases.xlsx
+++ b/SampleProject/src/main/resources/Testcases.xlsx
@@ -8,14 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="AllTcsEnabled" sheetId="2" r:id="rId2"/>
+    <sheet name="11TcsEnabled" sheetId="3" r:id="rId3"/>
+    <sheet name="7TcsEnabled" sheetId="4" r:id="rId4"/>
+    <sheet name="DivTcs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="45">
   <si>
     <t>TC_001</t>
   </si>
@@ -426,6 +429,10 @@
 {SettingsLinkDisplayed} VerifyEqual true
 Quit browser
 </t>
+  </si>
+  <si>
+    <t>Divide 10 by 5 Assign {Quotient}
+Print {Quotient}</t>
   </si>
 </sst>
 </file>
@@ -792,7 +799,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="409.5" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -814,7 +821,7 @@
     </row>
     <row r="3" spans="1:3" ht="209.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -836,7 +843,7 @@
     </row>
     <row r="5" spans="1:3" ht="225">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -858,7 +865,7 @@
     </row>
     <row r="7" spans="1:3" ht="135">
       <c r="A7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>14</v>
@@ -869,7 +876,7 @@
     </row>
     <row r="8" spans="1:3" ht="255">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>16</v>
@@ -880,7 +887,7 @@
     </row>
     <row r="9" spans="1:3" ht="183" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>18</v>
@@ -891,7 +898,7 @@
     </row>
     <row r="10" spans="1:3" ht="165">
       <c r="A10" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>20</v>
@@ -1012,7 +1019,7 @@
     </row>
     <row r="21" spans="1:3" ht="195">
       <c r="A21" s="5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>42</v>
@@ -1028,6 +1035,258 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="143" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="409.5" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="210">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="209.25" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="300">
+      <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="225">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="225">
+      <c r="A6" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="135">
+      <c r="A7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="255">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="183" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="165">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="168.75" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="123" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="123" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="198.75" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="209.25" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="256.5" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="168" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="196.5" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="140.25" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="225.75" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="195">
+      <c r="A21" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -1044,7 +1303,7 @@
   <sheetData>
     <row r="1" spans="1:3" ht="409.5" customHeight="1">
       <c r="A1" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1066,7 +1325,7 @@
     </row>
     <row r="3" spans="1:3" ht="209.25" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -1088,7 +1347,7 @@
     </row>
     <row r="5" spans="1:3" ht="225">
       <c r="A5" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -1110,7 +1369,7 @@
     </row>
     <row r="7" spans="1:3" ht="135">
       <c r="A7" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>14</v>
@@ -1121,7 +1380,7 @@
     </row>
     <row r="8" spans="1:3" ht="255">
       <c r="A8" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>16</v>
@@ -1132,7 +1391,7 @@
     </row>
     <row r="9" spans="1:3" ht="183" customHeight="1">
       <c r="A9" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>18</v>
@@ -1143,7 +1402,7 @@
     </row>
     <row r="10" spans="1:3" ht="165">
       <c r="A10" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>20</v>
@@ -1187,7 +1446,7 @@
     </row>
     <row r="14" spans="1:3" ht="198.75" customHeight="1">
       <c r="A14" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>28</v>
@@ -1220,7 +1479,7 @@
     </row>
     <row r="17" spans="1:3" ht="168" customHeight="1">
       <c r="A17" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>34</v>
@@ -1231,7 +1490,7 @@
     </row>
     <row r="18" spans="1:3" ht="196.5" customHeight="1">
       <c r="A18" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>36</v>
@@ -1274,7 +1533,519 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="143" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="409.5" customHeight="1">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="210">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="209.25" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="300">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="225">
+      <c r="A5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="225">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="135">
+      <c r="A7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="255">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="183" customHeight="1">
+      <c r="A9" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="165">
+      <c r="A10" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="168.75" customHeight="1">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="123" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="123" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="198.75" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="209.25" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="256.5" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="168" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="196.5" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="140.25" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="225.75" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="195">
+      <c r="A21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="143" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="409.5" customHeight="1">
+      <c r="A2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="210">
+      <c r="A3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="209.25" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="300">
+      <c r="A5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="225">
+      <c r="A6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="225">
+      <c r="A7" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="135">
+      <c r="A8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="255">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="183" customHeight="1">
+      <c r="A10" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="165">
+      <c r="A11" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="168.75" customHeight="1">
+      <c r="A12" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="123" customHeight="1">
+      <c r="A13" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="123" customHeight="1">
+      <c r="A14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="198.75" customHeight="1">
+      <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="209.25" customHeight="1">
+      <c r="A16" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="256.5" customHeight="1">
+      <c r="A17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="168" customHeight="1">
+      <c r="A18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="196.5" customHeight="1">
+      <c r="A19" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="140.25" customHeight="1">
+      <c r="A20" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="225.75" customHeight="1">
+      <c r="A21" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="195">
+      <c r="A22" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>